<commit_message>
new runs and little corrections
</commit_message>
<xml_diff>
--- a/slim_gsgp/consolidated_results_slim_oms_no_simplif.xlsx
+++ b/slim_gsgp/consolidated_results_slim_oms_no_simplif.xlsx
@@ -514,32 +514,32 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>6.58099 (15.62859)</t>
+          <t>6.71752 (20.45728)</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>24.26351 (36.22734)</t>
+          <t>23.27934 (33.00996)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>5.27834 (0.40593)</t>
+          <t>5.24107 (0.63219)</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>5.83879 (2.88445)</t>
+          <t>6.11062 (4.69217)</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>4.89212 (0.42016)</t>
+          <t>4.82583 (0.38435)</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>4.87734 (0.32548)</t>
+          <t>4.80051 (0.27714)</t>
         </is>
       </c>
     </row>
@@ -556,7 +556,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>670.29806 (466.79459)</t>
+          <t>670.41064 (466.62834)</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -566,7 +566,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>619.07061 (446.19282)</t>
+          <t>619.05834 (446.21035)</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -576,7 +576,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>593.99928 (435.24603)</t>
+          <t>593.99094 (435.25773)</t>
         </is>
       </c>
     </row>
@@ -588,32 +588,32 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>28.83807 (29.61919)</t>
+          <t>29.08046 (29.22538)</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>39.93259 (18.83271)</t>
+          <t>39.72433 (18.85535)</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>27.18933 (1.27957)</t>
+          <t>27.06833 (1.16061)</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>27.00752 (0.88950)</t>
+          <t>26.99933 (0.83115)</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>26.43062 (1.26583)</t>
+          <t>26.51568 (1.05829)</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>26.46471 (0.82702)</t>
+          <t>26.47794 (0.83159)</t>
         </is>
       </c>
     </row>
@@ -625,32 +625,32 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>5.81082 (1.36520)</t>
+          <t>5.83208 (2.08294)</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>8.46102 (6.87288)</t>
+          <t>7.88165 (4.87282)</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>5.14206 (0.61580)</t>
+          <t>5.09328 (0.61902)</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>5.21153 (0.58630)</t>
+          <t>5.15164 (0.40903)</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>4.83394 (0.53587)</t>
+          <t>4.84046 (0.35306)</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>4.88085 (0.32817)</t>
+          <t>4.88376 (0.30932)</t>
         </is>
       </c>
     </row>
@@ -662,32 +662,32 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>0.30089 (0.06486)</t>
+          <t>0.30949 (0.06999)</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>0.37488 (0.16838)</t>
+          <t>0.41757 (0.40102)</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>0.26751 (0.01874)</t>
+          <t>0.26775 (0.02277)</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>0.26543 (0.01559)</t>
+          <t>0.26726 (0.01681)</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>0.25322 (0.01557)</t>
+          <t>0.25447 (0.02245)</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>0.25448 (0.01347)</t>
+          <t>0.25572 (0.01549)</t>
         </is>
       </c>
     </row>
@@ -699,32 +699,32 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>7.94865 (1.52146)</t>
+          <t>7.68856 (0.71513)</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>10.24640 (5.03335)</t>
+          <t>9.16899 (3.93093)</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>7.32448 (0.76224)</t>
+          <t>7.16109 (0.65827)</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>7.15442 (0.58789)</t>
+          <t>7.16151 (0.60242)</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>6.99769 (0.72792)</t>
+          <t>6.99845 (0.57256)</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>6.89968 (0.50955)</t>
+          <t>6.92822 (0.49268)</t>
         </is>
       </c>
     </row>
@@ -736,32 +736,32 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>12.72642 (7.05545)</t>
+          <t>11.96134 (2.84296)</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>16.70548 (9.51418)</t>
+          <t>16.12530 (10.38777)</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>9.66120 (1.54750)</t>
+          <t>9.66221 (1.49875)</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>9.81616 (1.34017)</t>
+          <t>9.90169 (1.42507)</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>8.51004 (0.72763)</t>
+          <t>8.61869 (1.01351)</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>8.55024 (0.49516)</t>
+          <t>8.67738 (0.60967)</t>
         </is>
       </c>
     </row>
@@ -773,32 +773,32 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>72.81044 (6.38284)</t>
+          <t>72.31878 (5.48809)</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>77.66222 (13.80355)</t>
+          <t>76.72873 (12.29246)</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>68.25628 (4.36716)</t>
+          <t>69.59370 (3.89383)</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>69.12126 (2.93129)</t>
+          <t>69.61714 (2.79044)</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>66.16328 (4.13848)</t>
+          <t>67.05992 (4.41288)</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>66.62147 (2.78227)</t>
+          <t>67.32312 (2.40176)</t>
         </is>
       </c>
     </row>
@@ -810,32 +810,32 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>3.92592 (0.88841)</t>
+          <t>3.84551 (0.70642)</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>6.77048 (6.63475)</t>
+          <t>4.43861 (1.74775)</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>3.56329 (0.31152)</t>
+          <t>3.46279 (0.25766)</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>3.63059 (0.30295)</t>
+          <t>3.55873 (0.25437)</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>3.41899 (0.23557)</t>
+          <t>3.36723 (0.23443)</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>3.43742 (0.22037)</t>
+          <t>3.40990 (0.19373)</t>
         </is>
       </c>
     </row>
@@ -847,32 +847,32 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>4.46334 (1.55021)</t>
+          <t>3.99845 (1.48963)</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>6.67742 (5.94409)</t>
+          <t>5.69818 (4.18613)</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>3.31134 (0.40816)</t>
+          <t>3.34729 (0.20900)</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>3.41838 (0.37292)</t>
+          <t>3.41231 (0.26843)</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>3.09725 (0.23151)</t>
+          <t>3.19786 (0.16602)</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>3.16880 (0.21921)</t>
+          <t>3.23272 (0.24554)</t>
         </is>
       </c>
     </row>
@@ -884,32 +884,32 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>1.35271 (0.06742)</t>
+          <t>1.33940 (0.06608)</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>1.35425 (0.08312)</t>
+          <t>1.37255 (0.11655)</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>1.31677 (0.05629)</t>
+          <t>1.32023 (0.06170)</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>1.32112 (0.04428)</t>
+          <t>1.32470 (0.04484)</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>1.30858 (0.05590)</t>
+          <t>1.30916 (0.05838)</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>1.31273 (0.04499)</t>
+          <t>1.31392 (0.04565)</t>
         </is>
       </c>
     </row>
@@ -921,32 +921,32 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>0.01433 (0.00108)</t>
+          <t>0.01426 (0.00088)</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>0.08084 (0.36242)</t>
+          <t>0.01439 (0.00151)</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>0.01376 (0.00072)</t>
+          <t>0.01374 (0.00090)</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>0.01381 (0.00055)</t>
+          <t>0.01373 (0.00056)</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>0.01361 (0.00072)</t>
+          <t>0.01350 (0.00077)</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>0.01368 (0.00052)</t>
+          <t>0.01353 (0.00050)</t>
         </is>
       </c>
     </row>
@@ -958,32 +958,32 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>10.37609 (0.22690)</t>
+          <t>10.38130 (4.28489)</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>13.51933 (7.28084)</t>
+          <t>14.83208 (8.07650)</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>10.22174 (0.16608)</t>
+          <t>10.21122 (0.19479)</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>10.21426 (0.13412)</t>
+          <t>10.20378 (0.16396)</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>10.17085 (0.13030)</t>
+          <t>10.13423 (0.19662)</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>10.15017 (0.12117)</t>
+          <t>10.13540 (0.13437)</t>
         </is>
       </c>
     </row>
@@ -995,32 +995,32 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>25.77833 (3.53059)</t>
+          <t>25.48668 (2.17097)</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>32.83683 (16.80365)</t>
+          <t>30.39991 (14.48980)</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>23.41174 (1.19948)</t>
+          <t>23.13975 (1.61183)</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>23.11115 (1.30901)</t>
+          <t>22.87139 (1.23050)</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>22.25205 (1.62370)</t>
+          <t>21.81446 (1.84119)</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>22.01281 (1.22565)</t>
+          <t>21.91546 (1.13883)</t>
         </is>
       </c>
     </row>
@@ -1032,32 +1032,32 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>87.63794 (24.78561)</t>
+          <t>85.10263 (21.80751)</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>86.51137 (20.46683)</t>
+          <t>88.24885 (23.89627)</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>76.25775 (12.53154)</t>
+          <t>75.18346 (16.19943)</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>73.47350 (14.48132)</t>
+          <t>73.48199 (15.02225)</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>72.23913 (14.89391)</t>
+          <t>73.14989 (14.63424)</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>70.53329 (14.26871)</t>
+          <t>70.73033 (14.31089)</t>
         </is>
       </c>
     </row>
@@ -1159,32 +1159,32 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>6.53892 (15.74641)</t>
+          <t>6.81853 (20.21270)</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>24.28394 (36.18732)</t>
+          <t>23.33073 (32.95875)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>5.27807 (0.78205)</t>
+          <t>5.27680 (0.52949)</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>5.85242 (2.97653)</t>
+          <t>6.17759 (4.74526)</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>4.95316 (0.50281)</t>
+          <t>4.84492 (0.24783)</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>4.88760 (0.33600)</t>
+          <t>4.82857 (0.27223)</t>
         </is>
       </c>
     </row>
@@ -1201,7 +1201,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>682.42090 (478.12130)</t>
+          <t>682.53388 (477.95535)</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -1211,7 +1211,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>630.56412 (458.90101)</t>
+          <t>630.54644 (458.92604)</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -1221,7 +1221,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>604.79234 (446.97844)</t>
+          <t>604.79182 (446.97912)</t>
         </is>
       </c>
     </row>
@@ -1233,32 +1233,32 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>31.47191 (29.46948)</t>
+          <t>31.66343 (27.66714)</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>41.92190 (18.83754)</t>
+          <t>40.84623 (17.93487)</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>29.95866 (2.42474)</t>
+          <t>29.38904 (3.59394)</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>29.86374 (2.33428)</t>
+          <t>29.45820 (2.55477)</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>29.75474 (2.47832)</t>
+          <t>29.77508 (3.51506)</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>30.02267 (2.26329)</t>
+          <t>29.82236 (2.61188)</t>
         </is>
       </c>
     </row>
@@ -1270,32 +1270,32 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>6.61083 (2.09317)</t>
+          <t>6.51226 (2.61024)</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>8.89302 (6.79297)</t>
+          <t>8.37022 (5.09193)</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>5.65311 (1.56169)</t>
+          <t>5.64010 (1.14199)</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>5.77383 (0.99547)</t>
+          <t>6.01577 (1.97971)</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>5.47843 (1.37116)</t>
+          <t>5.41143 (1.22731)</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>5.47069 (0.82938)</t>
+          <t>5.79972 (2.00541)</t>
         </is>
       </c>
     </row>
@@ -1307,32 +1307,32 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>0.31439 (0.08024)</t>
+          <t>0.32472 (0.07840)</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>0.38271 (0.17307)</t>
+          <t>0.42729 (0.39267)</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>0.26170 (0.02943)</t>
+          <t>0.27423 (0.03338)</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>0.26836 (0.02125)</t>
+          <t>0.27399 (0.03001)</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>0.25715 (0.02840)</t>
+          <t>0.25747 (0.02475)</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>0.25830 (0.01941)</t>
+          <t>0.26349 (0.02838)</t>
         </is>
       </c>
     </row>
@@ -1344,32 +1344,32 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>8.82121 (2.19212)</t>
+          <t>8.65202 (2.07601)</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>10.76562 (4.75999)</t>
+          <t>9.93406 (4.15458)</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>8.01983 (1.36927)</t>
+          <t>7.92593 (1.61271)</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>8.09138 (1.08612)</t>
+          <t>7.80095 (1.09025)</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>7.83533 (1.47602)</t>
+          <t>7.67524 (1.32750)</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>7.86223 (1.04110)</t>
+          <t>7.67514 (1.00338)</t>
         </is>
       </c>
     </row>
@@ -1381,32 +1381,32 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>13.51856 (7.38915)</t>
+          <t>11.86276 (4.16088)</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>16.58003 (9.50411)</t>
+          <t>15.87307 (10.14370)</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>9.36787 (1.33785)</t>
+          <t>9.44151 (1.00750)</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>9.73524 (1.54389)</t>
+          <t>9.83128 (1.50385)</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>8.45099 (0.98910)</t>
+          <t>8.43714 (0.76940)</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>8.56155 (0.73548)</t>
+          <t>8.58924 (0.80881)</t>
         </is>
       </c>
     </row>
@@ -1418,32 +1418,32 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>75.57742 (7.08030)</t>
+          <t>75.19671 (6.30916)</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>79.37807 (11.64598)</t>
+          <t>79.44725 (12.94730)</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>72.06516 (7.80951)</t>
+          <t>71.77593 (6.71199)</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>71.52302 (4.70274)</t>
+          <t>71.57778 (4.90964)</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>70.35466 (6.71753)</t>
+          <t>70.64701 (5.62843)</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>69.44008 (4.69788)</t>
+          <t>70.03450 (4.66779)</t>
         </is>
       </c>
     </row>
@@ -1455,32 +1455,32 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>4.09528 (1.06490)</t>
+          <t>4.01903 (0.70220)</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>6.85496 (6.52156)</t>
+          <t>4.48805 (1.75721)</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>3.72260 (0.38642)</t>
+          <t>3.63481 (0.55070)</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>3.72688 (0.36551)</t>
+          <t>3.66402 (0.43997)</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>3.58199 (0.54527)</t>
+          <t>3.55478 (0.47503)</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>3.58509 (0.36954)</t>
+          <t>3.53560 (0.34835)</t>
         </is>
       </c>
     </row>
@@ -1492,32 +1492,32 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>4.47943 (1.49942)</t>
+          <t>4.25407 (1.43382)</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>6.75431 (6.05433)</t>
+          <t>5.74214 (4.16606)</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>3.34585 (0.51060)</t>
+          <t>3.35905 (0.43431)</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>3.47658 (0.39113)</t>
+          <t>3.46467 (0.34618)</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>3.15862 (0.22737)</t>
+          <t>3.22830 (0.42775)</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>3.20459 (0.27917)</t>
+          <t>3.30218 (0.31866)</t>
         </is>
       </c>
     </row>
@@ -1529,32 +1529,32 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>1.43127 (0.14837)</t>
+          <t>1.46956 (0.17890)</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>1.67904 (1.33511)</t>
+          <t>1.69364 (1.32919)</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>1.43395 (0.12527)</t>
+          <t>1.43837 (0.15982)</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>1.67082 (1.33466)</t>
+          <t>1.67275 (1.33489)</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>1.44205 (0.12762)</t>
+          <t>1.44162 (0.16076)</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>1.67490 (1.33431)</t>
+          <t>1.68071 (1.33388)</t>
         </is>
       </c>
     </row>
@@ -1566,32 +1566,32 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>0.01488 (0.00208)</t>
+          <t>0.01531 (0.00174)</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>0.08114 (0.36213)</t>
+          <t>0.01512 (0.00193)</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>0.01453 (0.00176)</t>
+          <t>0.01476 (0.00108)</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>0.01425 (0.00113)</t>
+          <t>0.01468 (0.00114)</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>0.01438 (0.00159)</t>
+          <t>0.01474 (0.00133)</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>0.01412 (0.00108)</t>
+          <t>0.01477 (0.00154)</t>
         </is>
       </c>
     </row>
@@ -1603,32 +1603,32 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>10.43682 (0.31221)</t>
+          <t>10.39442 (4.15066)</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>13.57164 (7.29554)</t>
+          <t>14.85123 (8.08349)</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>10.27701 (0.27880)</t>
+          <t>10.29136 (0.28084)</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>10.26764 (0.18181)</t>
+          <t>10.26647 (0.21510)</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>10.20754 (0.21013)</t>
+          <t>10.21133 (0.23715)</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>10.20527 (0.16857)</t>
+          <t>10.19441 (0.18135)</t>
         </is>
       </c>
     </row>
@@ -1640,32 +1640,32 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>31.64841 (8.38779)</t>
+          <t>30.72467 (7.71389)</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>36.87517 (15.85672)</t>
+          <t>34.34471 (13.41555)</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>29.86512 (5.53666)</t>
+          <t>30.76472 (5.05157)</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>29.86156 (4.53114)</t>
+          <t>29.43047 (4.57451)</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>30.42635 (5.50824)</t>
+          <t>31.18511 (6.74186)</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>30.07258 (4.25548)</t>
+          <t>29.57433 (4.97215)</t>
         </is>
       </c>
     </row>
@@ -1677,32 +1677,32 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>98.03301 (30.04378)</t>
+          <t>98.13951 (21.02660)</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>94.20466 (26.76654)</t>
+          <t>94.83167 (27.28267)</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>83.85916 (34.97238)</t>
+          <t>86.99241 (32.01614)</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>82.64229 (23.76284)</t>
+          <t>81.47093 (25.92367)</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>81.73676 (34.56876)</t>
+          <t>83.01032 (34.23876)</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>80.45337 (24.89931)</t>
+          <t>79.67587 (25.38479)</t>
         </is>
       </c>
     </row>
@@ -1804,32 +1804,32 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>33.00000 (13.50000)</t>
+          <t>34.00000 (16.00000)</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>35.60000 (15.53772)</t>
+          <t>35.73333 (13.34408)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>45.00000 (15.00000)</t>
+          <t>45.00000 (17.50000)</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>46.80000 (16.68656)</t>
+          <t>45.73333 (13.56957)</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>63.00000 (20.00000)</t>
+          <t>67.00000 (18.50000)</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>68.53333 (18.38052)</t>
+          <t>68.33333 (15.44140)</t>
         </is>
       </c>
     </row>
@@ -1841,32 +1841,32 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>35.00000 (7.50000)</t>
+          <t>35.00000 (6.00000)</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>37.66667 (12.82598)</t>
+          <t>37.26667 (12.15683)</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>42.00000 (10.50000)</t>
+          <t>42.00000 (7.50000)</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>45.00000 (12.70352)</t>
+          <t>44.93333 (11.90170)</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>53.00000 (11.50000)</t>
+          <t>53.00000 (14.50000)</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>56.13333 (14.40961)</t>
+          <t>56.13333 (12.72178)</t>
         </is>
       </c>
     </row>
@@ -1878,12 +1878,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>27.00000 (1.50000)</t>
+          <t>27.00000 (4.00000)</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>30.20000 (8.68768)</t>
+          <t>30.20000 (10.60384)</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -1893,7 +1893,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>35.53333 (9.03531)</t>
+          <t>35.40000 (10.43072)</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -1903,7 +1903,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>44.13333 (10.04381)</t>
+          <t>44.33333 (10.05273)</t>
         </is>
       </c>
     </row>
@@ -1915,32 +1915,32 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>29.00000 (8.00000)</t>
+          <t>28.00000 (6.00000)</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>28.06667 (7.51520)</t>
+          <t>28.33333 (6.58804)</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>35.00000 (4.00000)</t>
+          <t>35.00000 (9.50000)</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>35.86667 (6.44731)</t>
+          <t>35.80000 (7.05838)</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>45.00000 (8.00000)</t>
+          <t>48.00000 (9.50000)</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>47.80000 (6.44553)</t>
+          <t>49.26667 (7.34816)</t>
         </is>
       </c>
     </row>
@@ -1952,32 +1952,32 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>27.00000 (9.00000)</t>
+          <t>27.00000 (5.50000)</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>29.06667 (8.47688)</t>
+          <t>29.40000 (6.89628)</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>33.00000 (9.50000)</t>
+          <t>33.00000 (6.00000)</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>34.86667 (7.55547)</t>
+          <t>34.73333 (7.00213)</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>45.00000 (8.00000)</t>
+          <t>45.00000 (6.00000)</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>46.80000 (7.09249)</t>
+          <t>47.26667 (6.36224)</t>
         </is>
       </c>
     </row>
@@ -1989,32 +1989,32 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>30.00000 (15.00000)</t>
+          <t>30.00000 (9.50000)</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>33.13333 (17.88803)</t>
+          <t>33.93333 (14.86243)</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>38.00000 (15.00000)</t>
+          <t>37.00000 (11.50000)</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>42.53333 (18.72990)</t>
+          <t>41.00000 (15.79175)</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>55.00000 (17.00000)</t>
+          <t>52.00000 (12.00000)</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>60.13333 (17.70785)</t>
+          <t>56.06667 (15.95453)</t>
         </is>
       </c>
     </row>
@@ -2026,32 +2026,32 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>28.00000 (11.50000)</t>
+          <t>30.00000 (11.00000)</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>28.73333 (8.94016)</t>
+          <t>30.06667 (12.66800)</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>36.00000 (9.50000)</t>
+          <t>38.00000 (9.50000)</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>36.66667 (7.70281)</t>
+          <t>39.00000 (12.52859)</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>50.00000 (12.00000)</t>
+          <t>51.00000 (10.00000)</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>52.00000 (8.61034)</t>
+          <t>53.86667 (13.33580)</t>
         </is>
       </c>
     </row>
@@ -2063,32 +2063,32 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>33.00000 (8.00000)</t>
+          <t>32.00000 (8.00000)</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>34.60000 (13.99901)</t>
+          <t>36.46667 (17.78751)</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>39.00000 (11.50000)</t>
+          <t>40.00000 (9.50000)</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>42.46667 (15.28518)</t>
+          <t>44.66667 (17.95845)</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>53.00000 (11.50000)</t>
+          <t>55.00000 (11.50000)</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>58.06667 (14.45787)</t>
+          <t>59.80000 (16.12537)</t>
         </is>
       </c>
     </row>
@@ -2100,32 +2100,32 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>27.00000 (7.50000)</t>
+          <t>29.00000 (7.50000)</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>30.13333 (11.40700)</t>
+          <t>30.73333 (11.91618)</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>34.00000 (9.50000)</t>
+          <t>37.00000 (6.00000)</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>36.06667 (11.05140)</t>
+          <t>39.06667 (12.07429)</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>49.00000 (8.00000)</t>
+          <t>52.00000 (9.50000)</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>51.46667 (13.14831)</t>
+          <t>53.73333 (13.43678)</t>
         </is>
       </c>
     </row>
@@ -2137,32 +2137,32 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>29.00000 (8.00000)</t>
+          <t>31.00000 (8.00000)</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>30.13333 (13.00062)</t>
+          <t>32.26667 (12.80607)</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>37.00000 (9.50000)</t>
+          <t>37.00000 (7.50000)</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>37.93333 (12.03138)</t>
+          <t>39.93333 (12.25852)</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>53.00000 (13.00000)</t>
+          <t>53.00000 (13.50000)</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>55.00000 (12.64911)</t>
+          <t>56.40000 (15.26004)</t>
         </is>
       </c>
     </row>
@@ -2174,32 +2174,32 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>27.00000 (4.00000)</t>
+          <t>30.00000 (4.00000)</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>29.33333 (5.33261)</t>
+          <t>33.86667 (14.95449)</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>34.00000 (4.00000)</t>
+          <t>35.00000 (7.50000)</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>35.46667 (5.24393)</t>
+          <t>40.73333 (15.37336)</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>43.00000 (4.00000)</t>
+          <t>45.00000 (10.00000)</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>44.00000 (4.35494)</t>
+          <t>50.40000 (15.82795)</t>
         </is>
       </c>
     </row>
@@ -2211,32 +2211,32 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>25.00000 (10.00000)</t>
+          <t>29.00000 (11.50000)</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>27.80000 (5.32010)</t>
+          <t>28.06667 (8.34982)</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>32.00000 (9.50000)</t>
+          <t>38.00000 (8.00000)</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>33.26667 (5.98235)</t>
+          <t>37.20000 (7.35972)</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>52.00000 (11.50000)</t>
+          <t>57.00000 (10.00000)</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>51.20000 (9.19295)</t>
+          <t>56.13333 (8.59323)</t>
         </is>
       </c>
     </row>
@@ -2248,32 +2248,32 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>29.00000 (6.00000)</t>
+          <t>27.00000 (6.00000)</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>28.46667 (4.13341)</t>
+          <t>28.66667 (7.35472)</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>35.00000 (4.00000)</t>
+          <t>35.00000 (6.00000)</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>35.06667 (4.94057)</t>
+          <t>34.86667 (8.10165)</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>47.00000 (6.00000)</t>
+          <t>45.00000 (7.50000)</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>46.60000 (5.28890)</t>
+          <t>47.80000 (9.03022)</t>
         </is>
       </c>
     </row>
@@ -2285,22 +2285,22 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>27.00000 (7.00000)</t>
+          <t>27.00000 (4.00000)</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>31.86667 (15.25583)</t>
+          <t>31.86667 (14.92679)</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>34.00000 (4.00000)</t>
+          <t>33.00000 (4.00000)</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>37.73333 (15.63800)</t>
+          <t>37.80000 (15.21886)</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -2310,7 +2310,7 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>45.66667 (15.73341)</t>
+          <t>45.66667 (15.58366)</t>
         </is>
       </c>
     </row>
@@ -2327,27 +2327,27 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>26.26667 (4.44067)</t>
+          <t>26.13333 (4.59935)</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>31.00000 (5.50000)</t>
+          <t>31.00000 (4.00000)</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>32.06667 (4.86319)</t>
+          <t>31.60000 (4.27180)</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>41.00000 (3.50000)</t>
+          <t>41.00000 (2.00000)</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>41.20000 (3.68969)</t>
+          <t>40.93333 (3.21562)</t>
         </is>
       </c>
     </row>

</xml_diff>